<commit_message>
+velocity and position ploting for position_nodes determine;+calibration;
</commit_message>
<xml_diff>
--- a/communicate_with_basis_station_in_matlab/calibrations/calibration_results.xlsx
+++ b/communicate_with_basis_station_in_matlab/calibrations/calibration_results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="30">
   <si>
     <t>x</t>
   </si>
@@ -244,6 +244,24 @@
   </si>
   <si>
     <t>0x6E6E</t>
+  </si>
+  <si>
+    <t>trimmean(10)</t>
+  </si>
+  <si>
+    <t>mad(0)</t>
+  </si>
+  <si>
+    <t>700cm</t>
+  </si>
+  <si>
+    <t>f(x) = p1*x + p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1 =       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2 =        </t>
   </si>
 </sst>
 </file>
@@ -287,7 +305,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,8 +324,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -330,11 +366,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -345,7 +396,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -652,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
@@ -965,330 +1026,626 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Z16"/>
+  <dimension ref="B1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="1"/>
+    <col min="1" max="4" width="9.140625" style="6"/>
+    <col min="5" max="5" width="8.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="6" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="6"/>
+    <col min="10" max="11" width="9.140625" style="8"/>
+    <col min="12" max="12" width="3.42578125" style="6" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="6"/>
+    <col min="15" max="16" width="9.140625" style="8"/>
+    <col min="17" max="17" width="3.7109375" style="6" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="6"/>
+    <col min="20" max="21" width="9.140625" style="8"/>
+    <col min="22" max="22" width="2.85546875" style="6" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="6"/>
+    <col min="25" max="26" width="9.140625" style="8"/>
+    <col min="27" max="27" width="5" style="13" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="13"/>
+    <col min="29" max="29" width="9.140625" style="6"/>
+    <col min="30" max="31" width="9.140625" style="14"/>
+    <col min="32" max="32" width="5" style="6" customWidth="1"/>
+    <col min="33" max="34" width="9.140625" style="6"/>
+    <col min="35" max="35" width="1.5703125" style="6" customWidth="1"/>
+    <col min="36" max="37" width="9.140625" style="6"/>
+    <col min="38" max="38" width="1.140625" style="6" customWidth="1"/>
+    <col min="39" max="39" width="9.140625" style="7"/>
+    <col min="40" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="2:40">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AB1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:24">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:40">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="E2" t="s">
+      <c r="C2" s="7"/>
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Y2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AC2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AD2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AH2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" ht="15.75" thickBot="1">
-      <c r="B3" t="s">
+      <c r="AJ2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:40">
+      <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3">
-        <v>304.71764705882401</v>
-      </c>
-      <c r="I3">
-        <v>14.7288515406162</v>
-      </c>
-      <c r="K3">
-        <v>390.29927007299301</v>
-      </c>
-      <c r="L3">
-        <v>20.064190639759602</v>
-      </c>
-      <c r="N3">
-        <v>523.25</v>
-      </c>
-      <c r="O3">
-        <v>232.210526315789</v>
-      </c>
-      <c r="Q3">
-        <v>677.27272727272702</v>
-      </c>
-      <c r="R3">
-        <v>360.01671891326998</v>
-      </c>
-    </row>
-    <row r="4" spans="2:24" ht="77.25" thickBot="1">
-      <c r="C4" t="s">
+      <c r="H3" s="6">
+        <v>300.47301587301598</v>
+      </c>
+      <c r="I3" s="6">
+        <v>20.281912850065702</v>
+      </c>
+      <c r="J3" s="8">
+        <v>300.44169611307399</v>
+      </c>
+      <c r="K3" s="8">
+        <v>3.6247518266565701</v>
+      </c>
+      <c r="M3" s="6">
+        <v>407.55657492354698</v>
+      </c>
+      <c r="N3" s="6">
+        <v>99.732628985955301</v>
+      </c>
+      <c r="O3" s="8">
+        <v>408.06462585034001</v>
+      </c>
+      <c r="P3" s="8">
+        <v>7.78219192174243</v>
+      </c>
+      <c r="R3" s="6">
+        <v>518.29591836734699</v>
+      </c>
+      <c r="S3" s="6">
+        <v>52.242777179014404</v>
+      </c>
+      <c r="T3" s="8">
+        <v>517.46981132075496</v>
+      </c>
+      <c r="U3" s="8">
+        <v>4.0200263778981098</v>
+      </c>
+      <c r="W3" s="6">
+        <v>632.57894736842104</v>
+      </c>
+      <c r="X3" s="6">
+        <v>7.96976483762597</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>632.576470588235</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>2.2260387811634401</v>
+      </c>
+      <c r="AB3" s="13">
+        <v>717.92</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>5.5610810810810802</v>
+      </c>
+      <c r="AD3" s="14">
+        <v>717.89552238806004</v>
+      </c>
+      <c r="AE3" s="14">
+        <v>1.8474666666666699</v>
+      </c>
+      <c r="AM3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:40" ht="76.5">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="2:24">
-      <c r="H5" s="6">
+      <c r="E4" s="10"/>
+      <c r="H4" s="6">
+        <v>3.07749819748111</v>
+      </c>
+      <c r="O4" s="6">
+        <v>4.1618602105793503</v>
+      </c>
+      <c r="T4" s="6">
+        <v>5.2641794589420696</v>
+      </c>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="6">
+        <v>6.4239442881612101</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>89.73</v>
+      </c>
+      <c r="AN4" s="7">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:40">
+      <c r="H5" s="11">
         <v>349.26373626373601</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="11">
         <v>4.3963369963369896</v>
       </c>
     </row>
-    <row r="6" spans="2:24" ht="15.75" thickBot="1">
-      <c r="B6" t="s">
+    <row r="6" spans="2:40">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="H6">
-        <v>341.54117647058803</v>
-      </c>
-      <c r="I6">
-        <v>19.679831932773101</v>
-      </c>
-      <c r="K6">
-        <v>444.86029411764702</v>
-      </c>
-      <c r="L6">
-        <v>6.1951525054466297</v>
-      </c>
-      <c r="N6">
-        <v>557.88118811881202</v>
-      </c>
-      <c r="O6">
-        <v>158.505742574257</v>
-      </c>
-      <c r="Q6">
-        <v>658.22727272727298</v>
-      </c>
-      <c r="R6">
-        <v>9.0282131661441891</v>
-      </c>
-    </row>
-    <row r="7" spans="2:24" ht="77.25" thickBot="1">
-      <c r="C7" t="s">
+      <c r="E6" s="12"/>
+      <c r="H6" s="6">
+        <v>324.00623052959497</v>
+      </c>
+      <c r="I6" s="6">
+        <v>119.84371105919</v>
+      </c>
+      <c r="J6" s="8">
+        <v>323.30449826989599</v>
+      </c>
+      <c r="K6" s="8">
+        <v>9.2864199687503408</v>
+      </c>
+      <c r="M6" s="6">
+        <v>437.18320610686999</v>
+      </c>
+      <c r="N6" s="6">
+        <v>19.388402549197998</v>
+      </c>
+      <c r="O6" s="8">
+        <v>436.89303904923599</v>
+      </c>
+      <c r="P6" s="8">
+        <v>3.3383369267525902</v>
+      </c>
+      <c r="R6" s="6">
+        <v>550.568253968254</v>
+      </c>
+      <c r="S6" s="6">
+        <v>38.8180684886566</v>
+      </c>
+      <c r="T6" s="8">
+        <v>549.65669014084494</v>
+      </c>
+      <c r="U6" s="8">
+        <v>3.00384983623076</v>
+      </c>
+      <c r="W6" s="6">
+        <v>653.87368421052599</v>
+      </c>
+      <c r="X6" s="6">
+        <v>3.21791713325868</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>653.94117647058795</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>1.3990027700831</v>
+      </c>
+      <c r="AB6" s="13">
+        <v>744.96385542168696</v>
+      </c>
+      <c r="AC6" s="6">
+        <v>8.3523361739641508</v>
+      </c>
+      <c r="AD6" s="14">
+        <v>744.98666666666702</v>
+      </c>
+      <c r="AE6" s="14">
+        <v>2.1605457976484299</v>
+      </c>
+    </row>
+    <row r="7" spans="2:40" ht="76.5">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:24">
-      <c r="H8" s="6">
+      <c r="AM7" s="7">
+        <v>90.42</v>
+      </c>
+      <c r="AN7" s="6">
+        <v>5.5309999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40">
+      <c r="H8" s="11">
         <v>252.963636363636</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="11">
         <v>14.294949494949501</v>
       </c>
     </row>
-    <row r="9" spans="2:24" ht="15.75" thickBot="1">
-      <c r="B9" t="s">
+    <row r="9" spans="2:40">
+      <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="H9">
-        <v>293.917647058824</v>
-      </c>
-      <c r="I9">
-        <v>35.385994397759099</v>
-      </c>
-      <c r="K9">
-        <v>398.49635036496397</v>
-      </c>
-      <c r="L9">
-        <v>108.663589523401</v>
-      </c>
-      <c r="N9">
-        <v>499.29113924050603</v>
-      </c>
-      <c r="O9">
-        <v>17.2090230444661</v>
-      </c>
-      <c r="Q9">
-        <v>603.17045454545496</v>
-      </c>
-      <c r="R9">
-        <v>7.6142894461859996</v>
-      </c>
-    </row>
-    <row r="10" spans="2:24" ht="92.25" thickBot="1">
-      <c r="C10" t="s">
+      <c r="E9" s="12"/>
+      <c r="H9" s="6">
+        <v>287.35135135135101</v>
+      </c>
+      <c r="I9" s="6">
+        <v>59.062574438845601</v>
+      </c>
+      <c r="J9" s="8">
+        <v>287.327067669173</v>
+      </c>
+      <c r="K9" s="8">
+        <v>6.3175675675675498</v>
+      </c>
+      <c r="M9" s="6">
+        <v>403.14150943396203</v>
+      </c>
+      <c r="N9" s="6">
+        <v>90.896478977863694</v>
+      </c>
+      <c r="O9" s="8">
+        <v>402.81818181818198</v>
+      </c>
+      <c r="P9" s="8">
+        <v>7.1394921086982199</v>
+      </c>
+      <c r="R9" s="6">
+        <v>501.72805507745301</v>
+      </c>
+      <c r="S9" s="6">
+        <v>13.591435693513001</v>
+      </c>
+      <c r="T9" s="8">
+        <v>501.74187380497102</v>
+      </c>
+      <c r="U9" s="8">
+        <v>2.9602471849532401</v>
+      </c>
+      <c r="W9" s="6">
+        <v>618.66265060241005</v>
+      </c>
+      <c r="X9" s="6">
+        <v>5.0311489861886596</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>618.62666666666701</v>
+      </c>
+      <c r="Z9" s="8">
+        <v>1.7953258818406199</v>
+      </c>
+      <c r="AB9" s="13">
+        <v>716.58888888888896</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>7.6830212234706501</v>
+      </c>
+      <c r="AD9" s="14">
+        <v>716.52439024390196</v>
+      </c>
+      <c r="AE9" s="14">
+        <v>2.1967901234567901</v>
+      </c>
+    </row>
+    <row r="10" spans="2:40" ht="91.5">
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="2:24">
-      <c r="H11" s="6">
+      <c r="AM10" s="7">
+        <v>91.91</v>
+      </c>
+      <c r="AN10" s="6">
+        <v>23.44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:40">
+      <c r="H11" s="11">
         <v>317.622641509434</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="11">
         <v>6.6943396226415102</v>
       </c>
     </row>
-    <row r="12" spans="2:24" ht="15.75" thickBot="1">
-      <c r="B12" t="s">
+    <row r="12" spans="2:40">
+      <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="H12">
-        <v>313.058823529412</v>
-      </c>
-      <c r="I12">
-        <v>10.3179271708683</v>
-      </c>
-      <c r="K12">
-        <v>425.14598540146</v>
-      </c>
-      <c r="L12">
-        <v>10.493237440961799</v>
-      </c>
-      <c r="N12">
-        <v>530.65909090909099</v>
-      </c>
-      <c r="O12">
-        <v>16.165336571825101</v>
-      </c>
-      <c r="Q12">
-        <v>640.73863636363603</v>
-      </c>
-      <c r="R12">
-        <v>6.28722570532915</v>
-      </c>
-    </row>
-    <row r="13" spans="2:24" ht="92.25" thickBot="1">
-      <c r="C13" t="s">
+      <c r="E12" s="12"/>
+      <c r="H12" s="6">
+        <v>307.99256505576199</v>
+      </c>
+      <c r="I12" s="6">
+        <v>24.977556455639998</v>
+      </c>
+      <c r="J12" s="8">
+        <v>308.05349794238703</v>
+      </c>
+      <c r="K12" s="8">
+        <v>4.0149528060695499</v>
+      </c>
+      <c r="M12" s="6">
+        <v>421.58470764617698</v>
+      </c>
+      <c r="N12" s="6">
+        <v>11.0299760029894</v>
+      </c>
+      <c r="O12" s="8">
+        <v>421.472545757072</v>
+      </c>
+      <c r="P12" s="8">
+        <v>2.6066232251190602</v>
+      </c>
+      <c r="R12" s="6">
+        <v>525.31578947368405</v>
+      </c>
+      <c r="S12" s="6">
+        <v>21.6169942929615</v>
+      </c>
+      <c r="T12" s="8">
+        <v>525.110183639399</v>
+      </c>
+      <c r="U12" s="8">
+        <v>3.6492283339928702</v>
+      </c>
+      <c r="W12" s="6">
+        <v>649.45744680851101</v>
+      </c>
+      <c r="X12" s="6">
+        <v>7.6917181423015402</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>649.46428571428601</v>
+      </c>
+      <c r="Z12" s="8">
+        <v>2.2987777274785</v>
+      </c>
+      <c r="AB12" s="13">
+        <v>738.1</v>
+      </c>
+      <c r="AC12" s="6">
+        <v>3.7089887640449302</v>
+      </c>
+      <c r="AD12" s="14">
+        <v>738.19512195122002</v>
+      </c>
+      <c r="AE12" s="14">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:40" ht="91.5">
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="2:24">
-      <c r="H14" s="6">
+      <c r="AM13" s="7">
+        <v>89.84</v>
+      </c>
+      <c r="AN13" s="6">
+        <v>21.37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:40">
+      <c r="H14" s="11">
         <v>315.019230769231</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="11">
         <v>8.2937405731523395</v>
       </c>
     </row>
-    <row r="15" spans="2:24" ht="15.75" thickBot="1">
-      <c r="B15" t="s">
+    <row r="15" spans="2:40">
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="H15">
-        <v>314.35294117647101</v>
-      </c>
-      <c r="I15">
-        <v>12.46918767507</v>
-      </c>
-      <c r="K15">
-        <v>419.85401459854</v>
-      </c>
-      <c r="L15">
-        <v>10.2579433233147</v>
-      </c>
-      <c r="N15">
-        <v>521.65384615384596</v>
-      </c>
-      <c r="O15">
-        <v>9.9435564435564494</v>
-      </c>
-      <c r="Q15">
-        <v>624.17045454545496</v>
-      </c>
-      <c r="R15">
-        <v>8.8786572622779705</v>
-      </c>
-    </row>
-    <row r="16" spans="2:24" ht="77.25" thickBot="1">
-      <c r="C16" t="s">
+      <c r="E15" s="12"/>
+      <c r="H15" s="6">
+        <v>310.52012383900899</v>
+      </c>
+      <c r="I15" s="6">
+        <v>16.567140357287101</v>
+      </c>
+      <c r="J15" s="8">
+        <v>310.45017182130601</v>
+      </c>
+      <c r="K15" s="8">
+        <v>3.2194500091058198</v>
+      </c>
+      <c r="M15" s="6">
+        <v>418.446153846154</v>
+      </c>
+      <c r="N15" s="6">
+        <v>9.0487139978665603</v>
+      </c>
+      <c r="O15" s="8">
+        <v>418.53924914675798</v>
+      </c>
+      <c r="P15" s="8">
+        <v>2.2939644970414199</v>
+      </c>
+      <c r="R15" s="6">
+        <v>524.15608919382498</v>
+      </c>
+      <c r="S15" s="6">
+        <v>7.3072094215840799</v>
+      </c>
+      <c r="T15" s="8">
+        <v>524.299047619048</v>
+      </c>
+      <c r="U15" s="8">
+        <v>2.12688848418159</v>
+      </c>
+      <c r="W15" s="6">
+        <v>638.13684210526299</v>
+      </c>
+      <c r="X15" s="6">
+        <v>3.2257558790593501</v>
+      </c>
+      <c r="Y15" s="8">
+        <v>638.21176470588205</v>
+      </c>
+      <c r="Z15" s="8">
+        <v>1.39767313019391</v>
+      </c>
+      <c r="AB15" s="13">
+        <v>749.25806451612902</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>2.78476996298255</v>
+      </c>
+      <c r="AD15" s="14">
+        <v>717.92</v>
+      </c>
+      <c r="AE15" s="14">
+        <v>5.5610810810810802</v>
+      </c>
+    </row>
+    <row r="16" spans="2:40" ht="76.5">
+      <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="9" t="s">
         <v>18</v>
+      </c>
+      <c r="AM16" s="7">
+        <v>91.74</v>
+      </c>
+      <c r="AN16" s="6">
+        <v>15.89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+plot circle to see the result of the HTerm output data
</commit_message>
<xml_diff>
--- a/communicate_with_basis_station_in_matlab/calibrations/calibration_results.xlsx
+++ b/communicate_with_basis_station_in_matlab/calibrations/calibration_results.xlsx
@@ -1029,7 +1029,7 @@
   <dimension ref="B1:AN16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM4" sqref="AM4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1263,6 +1263,9 @@
       <c r="H4" s="6">
         <v>3.07749819748111</v>
       </c>
+      <c r="J4" s="8">
+        <v>3.07749819748111</v>
+      </c>
       <c r="O4" s="6">
         <v>4.1618602105793503</v>
       </c>

</xml_diff>